<commit_message>
Preparing for Alaska Merge
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Command</t>
   </si>
@@ -558,8 +558,8 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,16 +747,28 @@
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -857,8 +869,14 @@
       <c r="A23" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>30</v>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
guildMemberAdd (42+) System Check (Missing snowflake)
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
   <si>
     <t>Command</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>xks</t>
+  </si>
+  <si>
+    <t>Logging Event</t>
   </si>
 </sst>
 </file>
@@ -555,11 +558,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,6 +882,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Appended prefix to database
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
-  <si>
-    <t>Command</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="50">
   <si>
     <t>Role/Req</t>
   </si>
@@ -162,6 +159,21 @@
   </si>
   <si>
     <t>Limit</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Need Restructure</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
+    <t>s!</t>
+  </si>
+  <si>
+    <t>Complete 0.3.0.1b</t>
   </si>
 </sst>
 </file>
@@ -587,18 +599,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.109375" customWidth="1"/>
     <col min="5" max="5" width="35.44140625" customWidth="1"/>
     <col min="6" max="6" width="23.21875" customWidth="1"/>
@@ -606,415 +618,432 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
       <c r="D24" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the ping command to account for CSD/Bot Permissions.
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <t>Role/Req</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Testing Guild ID</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.2b</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,8 +711,11 @@
       <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>54</v>
+      <c r="F3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3">
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -776,8 +782,8 @@
       <c r="E7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>24</v>
+      <c r="F7" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Check Marco for citizen role
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
   <si>
     <t>Role/Req</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Complete 0.3.1.2b</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.4b</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,8 +785,11 @@
       <c r="E7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>54</v>
+      <c r="F7" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7">
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -816,8 +822,8 @@
       <c r="E9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>24</v>
+      <c r="F9" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changed the way XKS handles permissions.
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
   <si>
     <t>Role/Req</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Complete 0.3.1.5b</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.6b</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,8 +899,8 @@
       <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>54</v>
+      <c r="F13" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1057,8 +1060,8 @@
       <c r="E23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>24</v>
+      <c r="F23" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added a role check for rateme
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>Role/Req</t>
   </si>
@@ -188,6 +188,9 @@
     <t>Complete 0.3.0.16b</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Nested OR</t>
   </si>
   <si>
@@ -210,13 +213,22 @@
   </si>
   <si>
     <t>Complete 0.3.1.8b</t>
+  </si>
+  <si>
+    <t>Rushed</t>
+  </si>
+  <si>
+    <t>Untested In Full</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +257,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +340,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -354,6 +378,8 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -639,7 +665,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +728,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
@@ -711,7 +737,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>156</v>
@@ -724,6 +750,9 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="D4" s="8" t="s">
         <v>17</v>
       </c>
@@ -731,7 +760,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="G4">
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -782,7 +814,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G7">
         <v>192</v>
@@ -801,8 +833,8 @@
       <c r="E8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>24</v>
+      <c r="F8" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -819,7 +851,10 @@
         <v>18</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -890,7 +925,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13">
         <v>284</v>
@@ -903,6 +938,9 @@
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C14" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="D14" s="8" t="s">
         <v>17</v>
       </c>
@@ -910,7 +948,10 @@
         <v>21</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="G14">
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -932,7 +973,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>17</v>
@@ -1028,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>17</v>
@@ -1038,6 +1079,9 @@
       </c>
       <c r="F22" s="13" t="s">
         <v>53</v>
+      </c>
+      <c r="G22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1054,7 +1098,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G23">
         <v>311</v>

</xml_diff>

<commit_message>
0.3.1.10b Updates with Permissions
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
   <si>
     <t>Role/Req</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.9b</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +766,7 @@
         <v>62</v>
       </c>
       <c r="G4">
-        <v>340</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -833,8 +836,11 @@
       <c r="E8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>54</v>
+      <c r="F8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8">
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -873,8 +879,8 @@
       <c r="E10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>24</v>
+      <c r="F10" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
botrps now has citizen permissions
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Role/Req</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Complete 0.3.0.16b</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Nested OR</t>
   </si>
   <si>
@@ -221,17 +218,17 @@
     <t>Untested In Full</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Complete 0.3.1.9b</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.10b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,12 +257,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -366,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -381,7 +372,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -668,7 +658,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,7 +721,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
@@ -740,7 +730,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <v>156</v>
@@ -753,8 +743,8 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>64</v>
+      <c r="C4" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>17</v>
@@ -763,7 +753,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4">
         <v>348</v>
@@ -782,8 +772,11 @@
       <c r="E5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>24</v>
+      <c r="F5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5">
+        <v>486</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -817,7 +810,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7">
         <v>192</v>
@@ -837,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8">
         <v>377</v>
@@ -857,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9">
         <v>200</v>
@@ -879,8 +872,11 @@
       <c r="E10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>54</v>
+      <c r="F10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10">
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -931,7 +927,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13">
         <v>284</v>
@@ -944,8 +940,8 @@
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>63</v>
+      <c r="C14" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>17</v>
@@ -954,7 +950,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14">
         <v>310</v>
@@ -979,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>17</v>
@@ -1075,7 +1071,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>17</v>
@@ -1086,8 +1082,8 @@
       <c r="F22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G22" t="s">
-        <v>65</v>
+      <c r="G22">
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1104,7 +1100,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G23">
         <v>311</v>

</xml_diff>

<commit_message>
Separated help menu for Alaska
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +275,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -375,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -392,6 +399,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -677,7 +685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +790,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -828,7 +836,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -948,7 +956,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -968,7 +976,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -991,7 +999,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1133,7 +1141,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="2" t="s">

</xml_diff>

<commit_message>
Updated review sheet 0.3.1.16b
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="73">
   <si>
     <t>Role/Req</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>// Help</t>
+  </si>
+  <si>
+    <t>Appended</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -382,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -400,6 +409,7 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -681,11 +691,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,11 +706,10 @@
     <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -722,8 +731,11 @@
       <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -742,8 +754,11 @@
       <c r="F2" s="14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -765,8 +780,11 @@
       <c r="G3">
         <v>156</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -788,8 +806,11 @@
       <c r="G4">
         <v>348</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
@@ -811,8 +832,11 @@
       <c r="G5">
         <v>486</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -834,8 +858,11 @@
       <c r="G6">
         <v>529</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -854,8 +881,11 @@
       <c r="G7">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -874,8 +904,11 @@
       <c r="G8">
         <v>377</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -894,8 +927,11 @@
       <c r="G9">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -917,8 +953,11 @@
       <c r="G10">
         <v>386</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -934,8 +973,11 @@
       <c r="F11" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -954,8 +996,11 @@
       <c r="G12">
         <v>545</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>39</v>
       </c>
@@ -974,8 +1019,11 @@
       <c r="G13">
         <v>284</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
@@ -997,8 +1045,11 @@
       <c r="G14">
         <v>310</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
@@ -1011,8 +1062,11 @@
       <c r="F15" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1034,8 +1088,11 @@
       <c r="G16">
         <v>146</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -1048,8 +1105,11 @@
       <c r="F17" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1065,8 +1125,11 @@
       <c r="F18" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1085,8 +1148,11 @@
       <c r="G19">
         <v>535</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1102,8 +1168,11 @@
       <c r="F20" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1116,8 +1185,11 @@
       <c r="F21" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1139,8 +1211,11 @@
       <c r="G22">
         <v>452</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>49</v>
       </c>
@@ -1159,8 +1234,11 @@
       <c r="G23">
         <v>311</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1183,7 +1261,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1203,7 +1281,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
0.3.1.17b Modified help for Developers
</commit_message>
<xml_diff>
--- a/Alaska_Review.xlsx
+++ b/Alaska_Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="74">
   <si>
     <t>Role/Req</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Complete 0.3.1.17b</t>
   </si>
 </sst>
 </file>
@@ -695,7 +698,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,8 +973,8 @@
       <c r="E11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>24</v>
+      <c r="F11" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>71</v>
@@ -1088,7 +1091,7 @@
       <c r="G16">
         <v>146</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="14" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1148,7 +1151,7 @@
       <c r="G19">
         <v>535</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="14" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1168,7 +1171,7 @@
       <c r="F20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="14" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>